<commit_message>
update data and index
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mata Kuliah dan Praktikum\Semester 7\Asisten\NilaiWeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahmat\Documents\GitHub\NilaiLabDaselTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D39870E-B2A9-4344-924D-43E0E461E583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9FC08A-EEF5-4248-96AE-D5F8F0313CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="2520" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRAK TD" sheetId="1" r:id="rId1"/>
@@ -954,7 +954,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1069,6 +1069,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1138,7 +1146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1262,11 +1270,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1483,7 +1506,13 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1498,13 +1527,10 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1810,7 +1836,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1826,19 +1852,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="15.75" customHeight="1">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="80" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87" t="s">
+      <c r="D1" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="80" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1946,10 +1972,10 @@
       <c r="AN1" s="79" t="s">
         <v>299</v>
       </c>
-      <c r="AO1" s="87" t="s">
+      <c r="AO1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" s="87" t="s">
+      <c r="AP1" s="80" t="s">
         <v>6</v>
       </c>
       <c r="AQ1" s="1"/>
@@ -2100,11 +2126,11 @@
       <c r="AS2" s="8"/>
       <c r="AT2" s="8"/>
     </row>
-    <row r="3" spans="1:46" ht="15.75" customHeight="1">
+    <row r="3" spans="1:46" ht="15.75" customHeight="1" thickBot="1">
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="B3" s="89">
+      <c r="B3" s="82">
         <v>1192002</v>
       </c>
       <c r="C3" s="10">
@@ -2237,11 +2263,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="15.75" customHeight="1">
+    <row r="4" spans="1:46" ht="15.75" customHeight="1" thickBot="1">
       <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="88"/>
+      <c r="B4" s="90">
+        <v>1292022</v>
+      </c>
       <c r="C4" s="19">
         <v>3332230042</v>
       </c>
@@ -2372,11 +2400,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="15.75" customHeight="1">
+    <row r="5" spans="1:46" ht="15.75" customHeight="1" thickBot="1">
       <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="88"/>
+      <c r="B5" s="90">
+        <v>1121991</v>
+      </c>
       <c r="C5" s="19">
         <v>3332230045</v>
       </c>
@@ -2511,7 +2541,7 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="88"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="21">
         <v>3332230048</v>
       </c>
@@ -2646,7 +2676,7 @@
       <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="88"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="21">
         <v>3332230050</v>
       </c>
@@ -2781,7 +2811,7 @@
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="88"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="21">
         <v>3332230052</v>
       </c>
@@ -2916,7 +2946,7 @@
       <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="88"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="19">
         <v>3332230057</v>
       </c>
@@ -3051,7 +3081,7 @@
       <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="88"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="19">
         <v>3332230059</v>
       </c>
@@ -3186,7 +3216,7 @@
       <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" s="88"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="19">
         <v>3332230072</v>
       </c>
@@ -3321,7 +3351,7 @@
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="88"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="21">
         <v>3332230079</v>
       </c>
@@ -3456,7 +3486,7 @@
       <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="88"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="21">
         <v>3332230080</v>
       </c>
@@ -3591,7 +3621,7 @@
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="88"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="21">
         <v>3332230077</v>
       </c>
@@ -3721,10 +3751,10 @@
       <c r="AP14" s="18">
         <v>5</v>
       </c>
-      <c r="AQ14" s="86" t="s">
+      <c r="AQ14" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="AR14" s="80"/>
+      <c r="AR14" s="89"/>
       <c r="AS14" s="25" t="s">
         <v>7</v>
       </c>
@@ -3733,7 +3763,7 @@
       <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="88"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="19">
         <v>3332230041</v>
       </c>
@@ -3878,7 +3908,7 @@
       <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="88"/>
+      <c r="B16" s="81"/>
       <c r="C16" s="19">
         <v>3332230043</v>
       </c>
@@ -4023,7 +4053,7 @@
       <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="88"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="19">
         <v>3332230046</v>
       </c>
@@ -4168,7 +4198,7 @@
       <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="88"/>
+      <c r="B18" s="81"/>
       <c r="C18" s="21">
         <v>3332230047</v>
       </c>
@@ -4313,7 +4343,7 @@
       <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" s="88"/>
+      <c r="B19" s="81"/>
       <c r="C19" s="21">
         <v>3332230051</v>
       </c>
@@ -4458,7 +4488,7 @@
       <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" s="88"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="21">
         <v>3332230053</v>
       </c>
@@ -4603,7 +4633,7 @@
       <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" s="88"/>
+      <c r="B21" s="81"/>
       <c r="C21" s="19">
         <v>3332230060</v>
       </c>
@@ -4751,7 +4781,7 @@
       <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" s="88"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="19">
         <v>3332230061</v>
       </c>
@@ -4898,7 +4928,7 @@
       <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" s="88"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="19">
         <v>3332230063</v>
       </c>
@@ -5045,7 +5075,7 @@
       <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" s="88"/>
+      <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>3332230066</v>
       </c>
@@ -5177,10 +5207,10 @@
       <c r="AP24" s="18">
         <v>5</v>
       </c>
-      <c r="AQ24" s="81" t="s">
+      <c r="AQ24" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="AR24" s="82"/>
+      <c r="AR24" s="84"/>
       <c r="AS24" s="27">
         <f ca="1">SUM(AS15:AS23)</f>
         <v>115</v>
@@ -5190,7 +5220,7 @@
       <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" s="88"/>
+      <c r="B25" s="81"/>
       <c r="C25" s="21">
         <v>3332230070</v>
       </c>
@@ -5327,7 +5357,7 @@
       <c r="A26" s="9">
         <v>24</v>
       </c>
-      <c r="B26" s="88"/>
+      <c r="B26" s="81"/>
       <c r="C26" s="21">
         <v>3332230073</v>
       </c>
@@ -5464,7 +5494,7 @@
       <c r="A27" s="9">
         <v>25</v>
       </c>
-      <c r="B27" s="88"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="19">
         <v>3332230074</v>
       </c>
@@ -5601,7 +5631,7 @@
       <c r="A28" s="9">
         <v>26</v>
       </c>
-      <c r="B28" s="88"/>
+      <c r="B28" s="81"/>
       <c r="C28" s="19">
         <v>3332230056</v>
       </c>
@@ -5738,7 +5768,7 @@
       <c r="A29" s="9">
         <v>27</v>
       </c>
-      <c r="B29" s="88"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="19">
         <v>3332230082</v>
       </c>
@@ -5875,7 +5905,7 @@
       <c r="A30" s="9">
         <v>28</v>
       </c>
-      <c r="B30" s="88"/>
+      <c r="B30" s="81"/>
       <c r="C30" s="21">
         <v>3332230091</v>
       </c>
@@ -6012,7 +6042,7 @@
       <c r="A31" s="9">
         <v>29</v>
       </c>
-      <c r="B31" s="88"/>
+      <c r="B31" s="81"/>
       <c r="C31" s="21">
         <v>3332230113</v>
       </c>
@@ -6149,7 +6179,7 @@
       <c r="A32" s="9">
         <v>30</v>
       </c>
-      <c r="B32" s="88"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="21">
         <v>3332230001</v>
       </c>
@@ -6286,7 +6316,7 @@
       <c r="A33" s="9">
         <v>31</v>
       </c>
-      <c r="B33" s="88"/>
+      <c r="B33" s="81"/>
       <c r="C33" s="19">
         <v>3332230002</v>
       </c>
@@ -6423,7 +6453,7 @@
       <c r="A34" s="9">
         <v>32</v>
       </c>
-      <c r="B34" s="88"/>
+      <c r="B34" s="81"/>
       <c r="C34" s="19">
         <v>3332230003</v>
       </c>
@@ -6560,7 +6590,7 @@
       <c r="A35" s="9">
         <v>33</v>
       </c>
-      <c r="B35" s="88"/>
+      <c r="B35" s="81"/>
       <c r="C35" s="19">
         <v>3332230004</v>
       </c>
@@ -6697,7 +6727,7 @@
       <c r="A36" s="9">
         <v>34</v>
       </c>
-      <c r="B36" s="88"/>
+      <c r="B36" s="81"/>
       <c r="C36" s="21">
         <v>3332230005</v>
       </c>
@@ -6834,7 +6864,7 @@
       <c r="A37" s="9">
         <v>35</v>
       </c>
-      <c r="B37" s="88"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="21">
         <v>3332230006</v>
       </c>
@@ -6971,7 +7001,7 @@
       <c r="A38" s="9">
         <v>36</v>
       </c>
-      <c r="B38" s="88"/>
+      <c r="B38" s="81"/>
       <c r="C38" s="21">
         <v>3332230007</v>
       </c>
@@ -7108,7 +7138,7 @@
       <c r="A39" s="9">
         <v>37</v>
       </c>
-      <c r="B39" s="88"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="19">
         <v>3332230009</v>
       </c>
@@ -7245,7 +7275,7 @@
       <c r="A40" s="9">
         <v>38</v>
       </c>
-      <c r="B40" s="88"/>
+      <c r="B40" s="81"/>
       <c r="C40" s="19">
         <v>3332230010</v>
       </c>
@@ -7382,7 +7412,7 @@
       <c r="A41" s="9">
         <v>39</v>
       </c>
-      <c r="B41" s="88"/>
+      <c r="B41" s="81"/>
       <c r="C41" s="19">
         <v>3332230011</v>
       </c>
@@ -7519,7 +7549,7 @@
       <c r="A42" s="9">
         <v>40</v>
       </c>
-      <c r="B42" s="88"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="21">
         <v>3332230012</v>
       </c>
@@ -7656,7 +7686,7 @@
       <c r="A43" s="9">
         <v>41</v>
       </c>
-      <c r="B43" s="88"/>
+      <c r="B43" s="81"/>
       <c r="C43" s="21">
         <v>3332230013</v>
       </c>
@@ -7793,7 +7823,7 @@
       <c r="A44" s="9">
         <v>42</v>
       </c>
-      <c r="B44" s="88"/>
+      <c r="B44" s="81"/>
       <c r="C44" s="21">
         <v>3332230014</v>
       </c>
@@ -7930,7 +7960,7 @@
       <c r="A45" s="9">
         <v>43</v>
       </c>
-      <c r="B45" s="88"/>
+      <c r="B45" s="81"/>
       <c r="C45" s="19">
         <v>3332230015</v>
       </c>
@@ -8067,7 +8097,7 @@
       <c r="A46" s="9">
         <v>44</v>
       </c>
-      <c r="B46" s="88"/>
+      <c r="B46" s="81"/>
       <c r="C46" s="19">
         <v>3332230017</v>
       </c>
@@ -8204,7 +8234,7 @@
       <c r="A47" s="9">
         <v>45</v>
       </c>
-      <c r="B47" s="88"/>
+      <c r="B47" s="81"/>
       <c r="C47" s="19">
         <v>3332230019</v>
       </c>
@@ -8341,7 +8371,7 @@
       <c r="A48" s="9">
         <v>46</v>
       </c>
-      <c r="B48" s="88"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="21">
         <v>3332230020</v>
       </c>
@@ -8478,7 +8508,7 @@
       <c r="A49" s="9">
         <v>47</v>
       </c>
-      <c r="B49" s="88"/>
+      <c r="B49" s="81"/>
       <c r="C49" s="21">
         <v>3332230024</v>
       </c>
@@ -8615,7 +8645,7 @@
       <c r="A50" s="9">
         <v>48</v>
       </c>
-      <c r="B50" s="88"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="21">
         <v>3332230026</v>
       </c>
@@ -8752,7 +8782,7 @@
       <c r="A51" s="9">
         <v>49</v>
       </c>
-      <c r="B51" s="88"/>
+      <c r="B51" s="81"/>
       <c r="C51" s="19">
         <v>3332230027</v>
       </c>
@@ -8889,7 +8919,7 @@
       <c r="A52" s="9">
         <v>50</v>
       </c>
-      <c r="B52" s="88"/>
+      <c r="B52" s="81"/>
       <c r="C52" s="19">
         <v>3332230028</v>
       </c>
@@ -9026,7 +9056,7 @@
       <c r="A53" s="9">
         <v>51</v>
       </c>
-      <c r="B53" s="88"/>
+      <c r="B53" s="81"/>
       <c r="C53" s="19">
         <v>3332230029</v>
       </c>
@@ -9163,7 +9193,7 @@
       <c r="A54" s="9">
         <v>52</v>
       </c>
-      <c r="B54" s="88"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="21">
         <v>3332230030</v>
       </c>
@@ -9300,7 +9330,7 @@
       <c r="A55" s="9">
         <v>53</v>
       </c>
-      <c r="B55" s="88"/>
+      <c r="B55" s="81"/>
       <c r="C55" s="21">
         <v>3332230031</v>
       </c>
@@ -9437,7 +9467,7 @@
       <c r="A56" s="9">
         <v>54</v>
       </c>
-      <c r="B56" s="88"/>
+      <c r="B56" s="81"/>
       <c r="C56" s="21">
         <v>3332230032</v>
       </c>
@@ -9574,7 +9604,7 @@
       <c r="A57" s="9">
         <v>55</v>
       </c>
-      <c r="B57" s="88"/>
+      <c r="B57" s="81"/>
       <c r="C57" s="19">
         <v>3332230033</v>
       </c>
@@ -9711,7 +9741,7 @@
       <c r="A58" s="9">
         <v>56</v>
       </c>
-      <c r="B58" s="88"/>
+      <c r="B58" s="81"/>
       <c r="C58" s="19">
         <v>3332230034</v>
       </c>
@@ -9848,7 +9878,7 @@
       <c r="A59" s="9">
         <v>57</v>
       </c>
-      <c r="B59" s="88"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="19">
         <v>3332230035</v>
       </c>
@@ -9985,7 +10015,7 @@
       <c r="A60" s="9">
         <v>58</v>
       </c>
-      <c r="B60" s="88"/>
+      <c r="B60" s="81"/>
       <c r="C60" s="21">
         <v>3332230037</v>
       </c>
@@ -10122,7 +10152,7 @@
       <c r="A61" s="9">
         <v>59</v>
       </c>
-      <c r="B61" s="88"/>
+      <c r="B61" s="81"/>
       <c r="C61" s="21">
         <v>3332230039</v>
       </c>
@@ -10259,7 +10289,7 @@
       <c r="A62" s="9">
         <v>60</v>
       </c>
-      <c r="B62" s="88"/>
+      <c r="B62" s="81"/>
       <c r="C62" s="21">
         <v>3332230025</v>
       </c>
@@ -10396,7 +10426,7 @@
       <c r="A63" s="9">
         <v>61</v>
       </c>
-      <c r="B63" s="88"/>
+      <c r="B63" s="81"/>
       <c r="C63" s="19">
         <v>3332230124</v>
       </c>
@@ -10533,7 +10563,7 @@
       <c r="A64" s="9">
         <v>62</v>
       </c>
-      <c r="B64" s="88"/>
+      <c r="B64" s="81"/>
       <c r="C64" s="19">
         <v>3332230137</v>
       </c>
@@ -10670,7 +10700,7 @@
       <c r="A65" s="9">
         <v>63</v>
       </c>
-      <c r="B65" s="88"/>
+      <c r="B65" s="81"/>
       <c r="C65" s="19">
         <v>3332230127</v>
       </c>
@@ -10807,7 +10837,7 @@
       <c r="A66" s="9">
         <v>64</v>
       </c>
-      <c r="B66" s="88"/>
+      <c r="B66" s="81"/>
       <c r="C66" s="21">
         <v>3332230125</v>
       </c>
@@ -10944,7 +10974,7 @@
       <c r="A67" s="9">
         <v>65</v>
       </c>
-      <c r="B67" s="88"/>
+      <c r="B67" s="81"/>
       <c r="C67" s="21">
         <v>3332230126</v>
       </c>
@@ -11081,7 +11111,7 @@
       <c r="A68" s="9">
         <v>66</v>
       </c>
-      <c r="B68" s="88"/>
+      <c r="B68" s="81"/>
       <c r="C68" s="21">
         <v>3332230128</v>
       </c>
@@ -11218,7 +11248,7 @@
       <c r="A69" s="9">
         <v>67</v>
       </c>
-      <c r="B69" s="88"/>
+      <c r="B69" s="81"/>
       <c r="C69" s="19">
         <v>3332230129</v>
       </c>
@@ -11359,7 +11389,7 @@
       <c r="A70" s="9">
         <v>68</v>
       </c>
-      <c r="B70" s="88"/>
+      <c r="B70" s="81"/>
       <c r="C70" s="19">
         <v>3332230130</v>
       </c>
@@ -11496,7 +11526,7 @@
       <c r="A71" s="9">
         <v>69</v>
       </c>
-      <c r="B71" s="88"/>
+      <c r="B71" s="81"/>
       <c r="C71" s="19">
         <v>3332230133</v>
       </c>
@@ -11633,7 +11663,7 @@
       <c r="A72" s="9">
         <v>70</v>
       </c>
-      <c r="B72" s="88"/>
+      <c r="B72" s="81"/>
       <c r="C72" s="21">
         <v>3332230134</v>
       </c>
@@ -11770,7 +11800,7 @@
       <c r="A73" s="9">
         <v>71</v>
       </c>
-      <c r="B73" s="88"/>
+      <c r="B73" s="81"/>
       <c r="C73" s="21">
         <v>3332230081</v>
       </c>
@@ -11907,7 +11937,7 @@
       <c r="A74" s="9">
         <v>72</v>
       </c>
-      <c r="B74" s="88"/>
+      <c r="B74" s="81"/>
       <c r="C74" s="21">
         <v>3332230083</v>
       </c>
@@ -12044,7 +12074,7 @@
       <c r="A75" s="9">
         <v>73</v>
       </c>
-      <c r="B75" s="88"/>
+      <c r="B75" s="81"/>
       <c r="C75" s="19">
         <v>3332230084</v>
       </c>
@@ -12181,7 +12211,7 @@
       <c r="A76" s="9">
         <v>74</v>
       </c>
-      <c r="B76" s="88"/>
+      <c r="B76" s="81"/>
       <c r="C76" s="19">
         <v>3332230086</v>
       </c>
@@ -12318,7 +12348,7 @@
       <c r="A77" s="9">
         <v>75</v>
       </c>
-      <c r="B77" s="88"/>
+      <c r="B77" s="81"/>
       <c r="C77" s="19">
         <v>3332230087</v>
       </c>
@@ -12455,7 +12485,7 @@
       <c r="A78" s="9">
         <v>76</v>
       </c>
-      <c r="B78" s="88"/>
+      <c r="B78" s="81"/>
       <c r="C78" s="21">
         <v>3332230088</v>
       </c>
@@ -12592,7 +12622,7 @@
       <c r="A79" s="9">
         <v>77</v>
       </c>
-      <c r="B79" s="88"/>
+      <c r="B79" s="81"/>
       <c r="C79" s="21">
         <v>3332230089</v>
       </c>
@@ -12729,7 +12759,7 @@
       <c r="A80" s="9">
         <v>78</v>
       </c>
-      <c r="B80" s="88"/>
+      <c r="B80" s="81"/>
       <c r="C80" s="21">
         <v>3332230090</v>
       </c>
@@ -12866,7 +12896,7 @@
       <c r="A81" s="9">
         <v>79</v>
       </c>
-      <c r="B81" s="88"/>
+      <c r="B81" s="81"/>
       <c r="C81" s="19">
         <v>3332230092</v>
       </c>
@@ -13003,7 +13033,7 @@
       <c r="A82" s="9">
         <v>80</v>
       </c>
-      <c r="B82" s="88"/>
+      <c r="B82" s="81"/>
       <c r="C82" s="19">
         <v>3332230093</v>
       </c>
@@ -13140,7 +13170,7 @@
       <c r="A83" s="9">
         <v>81</v>
       </c>
-      <c r="B83" s="88"/>
+      <c r="B83" s="81"/>
       <c r="C83" s="19">
         <v>3332230094</v>
       </c>
@@ -13277,7 +13307,7 @@
       <c r="A84" s="9">
         <v>82</v>
       </c>
-      <c r="B84" s="88"/>
+      <c r="B84" s="81"/>
       <c r="C84" s="21">
         <v>3332230095</v>
       </c>
@@ -13414,7 +13444,7 @@
       <c r="A85" s="9">
         <v>83</v>
       </c>
-      <c r="B85" s="88"/>
+      <c r="B85" s="81"/>
       <c r="C85" s="21">
         <v>3332230096</v>
       </c>
@@ -13551,7 +13581,7 @@
       <c r="A86" s="9">
         <v>84</v>
       </c>
-      <c r="B86" s="88"/>
+      <c r="B86" s="81"/>
       <c r="C86" s="21">
         <v>3332230097</v>
       </c>
@@ -13688,7 +13718,7 @@
       <c r="A87" s="9">
         <v>85</v>
       </c>
-      <c r="B87" s="88"/>
+      <c r="B87" s="81"/>
       <c r="C87" s="19">
         <v>3332230098</v>
       </c>
@@ -13829,7 +13859,7 @@
       <c r="A88" s="9">
         <v>86</v>
       </c>
-      <c r="B88" s="88"/>
+      <c r="B88" s="81"/>
       <c r="C88" s="19">
         <v>3332230099</v>
       </c>
@@ -13970,7 +14000,7 @@
       <c r="A89" s="9">
         <v>87</v>
       </c>
-      <c r="B89" s="88"/>
+      <c r="B89" s="81"/>
       <c r="C89" s="19">
         <v>3332230101</v>
       </c>
@@ -14111,7 +14141,7 @@
       <c r="A90" s="9">
         <v>88</v>
       </c>
-      <c r="B90" s="88"/>
+      <c r="B90" s="81"/>
       <c r="C90" s="21">
         <v>3332230103</v>
       </c>
@@ -14252,7 +14282,7 @@
       <c r="A91" s="9">
         <v>89</v>
       </c>
-      <c r="B91" s="88"/>
+      <c r="B91" s="81"/>
       <c r="C91" s="21">
         <v>3332230104</v>
       </c>
@@ -14393,7 +14423,7 @@
       <c r="A92" s="9">
         <v>90</v>
       </c>
-      <c r="B92" s="88"/>
+      <c r="B92" s="81"/>
       <c r="C92" s="21">
         <v>3332230105</v>
       </c>
@@ -14533,7 +14563,7 @@
       <c r="A93" s="9">
         <v>91</v>
       </c>
-      <c r="B93" s="88"/>
+      <c r="B93" s="81"/>
       <c r="C93" s="19">
         <v>3332230108</v>
       </c>
@@ -14671,7 +14701,7 @@
       <c r="A94" s="9">
         <v>92</v>
       </c>
-      <c r="B94" s="88"/>
+      <c r="B94" s="81"/>
       <c r="C94" s="19">
         <v>3332230109</v>
       </c>
@@ -14808,7 +14838,7 @@
       <c r="A95" s="9">
         <v>93</v>
       </c>
-      <c r="B95" s="88"/>
+      <c r="B95" s="81"/>
       <c r="C95" s="19">
         <v>3332230110</v>
       </c>
@@ -14949,7 +14979,7 @@
       <c r="A96" s="9">
         <v>94</v>
       </c>
-      <c r="B96" s="88"/>
+      <c r="B96" s="81"/>
       <c r="C96" s="21">
         <v>3332230111</v>
       </c>
@@ -15090,7 +15120,7 @@
       <c r="A97" s="9">
         <v>95</v>
       </c>
-      <c r="B97" s="88"/>
+      <c r="B97" s="81"/>
       <c r="C97" s="21">
         <v>3332230112</v>
       </c>
@@ -15227,7 +15257,7 @@
       <c r="A98" s="9">
         <v>96</v>
       </c>
-      <c r="B98" s="88"/>
+      <c r="B98" s="81"/>
       <c r="C98" s="21">
         <v>3332230114</v>
       </c>
@@ -15368,7 +15398,7 @@
       <c r="A99" s="9">
         <v>97</v>
       </c>
-      <c r="B99" s="88"/>
+      <c r="B99" s="81"/>
       <c r="C99" s="19">
         <v>3332230115</v>
       </c>
@@ -15509,7 +15539,7 @@
       <c r="A100" s="9">
         <v>98</v>
       </c>
-      <c r="B100" s="88"/>
+      <c r="B100" s="81"/>
       <c r="C100" s="19">
         <v>3332230116</v>
       </c>
@@ -15650,7 +15680,7 @@
       <c r="A101" s="9">
         <v>99</v>
       </c>
-      <c r="B101" s="88"/>
+      <c r="B101" s="81"/>
       <c r="C101" s="19">
         <v>3332230118</v>
       </c>
@@ -15791,7 +15821,7 @@
       <c r="A102" s="9">
         <v>100</v>
       </c>
-      <c r="B102" s="88"/>
+      <c r="B102" s="81"/>
       <c r="C102" s="21">
         <v>3332230119</v>
       </c>
@@ -15928,7 +15958,7 @@
       <c r="A103" s="9">
         <v>101</v>
       </c>
-      <c r="B103" s="88"/>
+      <c r="B103" s="81"/>
       <c r="C103" s="21">
         <v>3332230100</v>
       </c>
@@ -16065,7 +16095,7 @@
       <c r="A104" s="9">
         <v>102</v>
       </c>
-      <c r="B104" s="88"/>
+      <c r="B104" s="81"/>
       <c r="C104" s="21">
         <v>3332230022</v>
       </c>
@@ -16202,7 +16232,7 @@
       <c r="A105" s="9">
         <v>103</v>
       </c>
-      <c r="B105" s="88"/>
+      <c r="B105" s="81"/>
       <c r="C105" s="19">
         <v>3332230023</v>
       </c>
@@ -16343,7 +16373,7 @@
       <c r="A106" s="9">
         <v>104</v>
       </c>
-      <c r="B106" s="88"/>
+      <c r="B106" s="81"/>
       <c r="C106" s="19">
         <v>3332230036</v>
       </c>
@@ -16484,7 +16514,7 @@
       <c r="A107" s="9">
         <v>105</v>
       </c>
-      <c r="B107" s="88"/>
+      <c r="B107" s="81"/>
       <c r="C107" s="19">
         <v>3332230038</v>
       </c>
@@ -16625,7 +16655,7 @@
       <c r="A108" s="9">
         <v>106</v>
       </c>
-      <c r="B108" s="88"/>
+      <c r="B108" s="81"/>
       <c r="C108" s="21">
         <v>3332230121</v>
       </c>
@@ -16766,7 +16796,7 @@
       <c r="A109" s="9">
         <v>107</v>
       </c>
-      <c r="B109" s="88"/>
+      <c r="B109" s="81"/>
       <c r="C109" s="21">
         <v>3332230131</v>
       </c>
@@ -16907,7 +16937,7 @@
       <c r="A110" s="9">
         <v>108</v>
       </c>
-      <c r="B110" s="88"/>
+      <c r="B110" s="81"/>
       <c r="C110" s="21">
         <v>3332230055</v>
       </c>
@@ -17048,7 +17078,7 @@
       <c r="A111" s="9">
         <v>109</v>
       </c>
-      <c r="B111" s="88"/>
+      <c r="B111" s="81"/>
       <c r="C111" s="19">
         <v>3332230049</v>
       </c>
@@ -17187,7 +17217,7 @@
       <c r="A112" s="9">
         <v>110</v>
       </c>
-      <c r="B112" s="88"/>
+      <c r="B112" s="81"/>
       <c r="C112" s="19">
         <v>3332230044</v>
       </c>
@@ -17328,7 +17358,7 @@
       <c r="A113" s="9">
         <v>111</v>
       </c>
-      <c r="B113" s="88"/>
+      <c r="B113" s="81"/>
       <c r="C113" s="19">
         <v>3332230054</v>
       </c>
@@ -17469,7 +17499,7 @@
       <c r="A114" s="9">
         <v>112</v>
       </c>
-      <c r="B114" s="88"/>
+      <c r="B114" s="81"/>
       <c r="C114" s="21">
         <v>3332230069</v>
       </c>
@@ -17610,7 +17640,7 @@
       <c r="A115" s="9">
         <v>113</v>
       </c>
-      <c r="B115" s="88"/>
+      <c r="B115" s="81"/>
       <c r="C115" s="21">
         <v>3332230008</v>
       </c>
@@ -17747,7 +17777,7 @@
       <c r="A116" s="9">
         <v>114</v>
       </c>
-      <c r="B116" s="88"/>
+      <c r="B116" s="81"/>
       <c r="C116" s="21">
         <v>3332230016</v>
       </c>
@@ -17888,7 +17918,7 @@
       <c r="A117" s="9">
         <v>115</v>
       </c>
-      <c r="B117" s="88"/>
+      <c r="B117" s="81"/>
       <c r="C117" s="19">
         <v>3332230018</v>
       </c>
@@ -18025,7 +18055,7 @@
       <c r="A118" s="9">
         <v>116</v>
       </c>
-      <c r="B118" s="88"/>
+      <c r="B118" s="81"/>
       <c r="C118" s="19">
         <v>3332230021</v>
       </c>
@@ -18164,7 +18194,7 @@
       <c r="A119" s="9">
         <v>117</v>
       </c>
-      <c r="B119" s="88"/>
+      <c r="B119" s="81"/>
       <c r="C119" s="19">
         <v>3332230058</v>
       </c>
@@ -18301,7 +18331,7 @@
       <c r="A120" s="9">
         <v>118</v>
       </c>
-      <c r="B120" s="88"/>
+      <c r="B120" s="81"/>
       <c r="C120" s="21">
         <v>3332230062</v>
       </c>
@@ -18438,7 +18468,7 @@
       <c r="A121" s="9">
         <v>119</v>
       </c>
-      <c r="B121" s="88"/>
+      <c r="B121" s="81"/>
       <c r="C121" s="21">
         <v>3332230064</v>
       </c>
@@ -18579,7 +18609,7 @@
       <c r="A122" s="9">
         <v>120</v>
       </c>
-      <c r="B122" s="88"/>
+      <c r="B122" s="81"/>
       <c r="C122" s="21">
         <v>3332230065</v>
       </c>
@@ -18720,7 +18750,7 @@
       <c r="A123" s="9">
         <v>121</v>
       </c>
-      <c r="B123" s="88"/>
+      <c r="B123" s="81"/>
       <c r="C123" s="19">
         <v>3332230067</v>
       </c>
@@ -18861,7 +18891,7 @@
       <c r="A124" s="9">
         <v>122</v>
       </c>
-      <c r="B124" s="88"/>
+      <c r="B124" s="81"/>
       <c r="C124" s="19">
         <v>3332230068</v>
       </c>
@@ -19001,7 +19031,7 @@
       <c r="A125" s="9">
         <v>123</v>
       </c>
-      <c r="B125" s="88"/>
+      <c r="B125" s="81"/>
       <c r="C125" s="19">
         <v>3332230071</v>
       </c>
@@ -19138,7 +19168,7 @@
       <c r="A126" s="9">
         <v>124</v>
       </c>
-      <c r="B126" s="88"/>
+      <c r="B126" s="81"/>
       <c r="C126" s="21">
         <v>3332230075</v>
       </c>
@@ -19268,15 +19298,15 @@
       <c r="AP126" s="18">
         <v>5</v>
       </c>
-      <c r="AQ126" s="83"/>
-      <c r="AR126" s="84"/>
+      <c r="AQ126" s="85"/>
+      <c r="AR126" s="86"/>
       <c r="AS126" s="40"/>
     </row>
     <row r="127" spans="1:46" ht="15.75" customHeight="1">
       <c r="A127" s="9">
         <v>125</v>
       </c>
-      <c r="B127" s="88"/>
+      <c r="B127" s="81"/>
       <c r="C127" s="21">
         <v>3332230078</v>
       </c>
@@ -19413,7 +19443,7 @@
       <c r="A128" s="9">
         <v>126</v>
       </c>
-      <c r="B128" s="88"/>
+      <c r="B128" s="81"/>
       <c r="C128" s="21">
         <v>3332230085</v>
       </c>
@@ -19552,7 +19582,7 @@
       <c r="A129" s="9">
         <v>127</v>
       </c>
-      <c r="B129" s="88"/>
+      <c r="B129" s="81"/>
       <c r="C129" s="19">
         <v>3332230102</v>
       </c>
@@ -19689,7 +19719,7 @@
       <c r="A130" s="9">
         <v>128</v>
       </c>
-      <c r="B130" s="88"/>
+      <c r="B130" s="81"/>
       <c r="C130" s="19">
         <v>3332230106</v>
       </c>
@@ -19829,7 +19859,7 @@
       <c r="A131" s="9">
         <v>129</v>
       </c>
-      <c r="B131" s="88"/>
+      <c r="B131" s="81"/>
       <c r="C131" s="19">
         <v>3332230107</v>
       </c>
@@ -19970,7 +20000,7 @@
       <c r="A132" s="9">
         <v>130</v>
       </c>
-      <c r="B132" s="88"/>
+      <c r="B132" s="81"/>
       <c r="C132" s="21">
         <v>3332230117</v>
       </c>
@@ -20107,7 +20137,7 @@
       <c r="A133" s="9">
         <v>131</v>
       </c>
-      <c r="B133" s="88"/>
+      <c r="B133" s="81"/>
       <c r="C133" s="21">
         <v>3332230120</v>
       </c>
@@ -20248,7 +20278,7 @@
       <c r="A134" s="9">
         <v>132</v>
       </c>
-      <c r="B134" s="88"/>
+      <c r="B134" s="81"/>
       <c r="C134" s="21">
         <v>3332230123</v>
       </c>
@@ -20387,7 +20417,7 @@
       <c r="A135" s="9">
         <v>133</v>
       </c>
-      <c r="B135" s="88"/>
+      <c r="B135" s="81"/>
       <c r="C135" s="19">
         <v>3332230132</v>
       </c>
@@ -20524,7 +20554,7 @@
       <c r="A136" s="9">
         <v>134</v>
       </c>
-      <c r="B136" s="88"/>
+      <c r="B136" s="81"/>
       <c r="C136" s="19">
         <v>3332230135</v>
       </c>
@@ -20661,7 +20691,7 @@
       <c r="A137" s="9">
         <v>135</v>
       </c>
-      <c r="B137" s="88"/>
+      <c r="B137" s="81"/>
       <c r="C137" s="19">
         <v>3332230136</v>
       </c>
@@ -20800,7 +20830,7 @@
       <c r="A138" s="9">
         <v>136</v>
       </c>
-      <c r="B138" s="88"/>
+      <c r="B138" s="81"/>
       <c r="C138" s="21">
         <v>3332210060</v>
       </c>
@@ -20937,7 +20967,7 @@
       <c r="A139" s="9">
         <v>137</v>
       </c>
-      <c r="B139" s="88"/>
+      <c r="B139" s="81"/>
       <c r="C139" s="21">
         <v>3332210068</v>
       </c>
@@ -21078,7 +21108,7 @@
       <c r="A140" s="9">
         <v>138</v>
       </c>
-      <c r="B140" s="88"/>
+      <c r="B140" s="81"/>
       <c r="C140" s="21">
         <v>3332210029</v>
       </c>
@@ -21215,7 +21245,7 @@
       <c r="A141" s="9">
         <v>139</v>
       </c>
-      <c r="B141" s="88"/>
+      <c r="B141" s="81"/>
       <c r="C141" s="19">
         <v>3332210080</v>
       </c>
@@ -21356,7 +21386,7 @@
       <c r="A142" s="9">
         <v>140</v>
       </c>
-      <c r="B142" s="88"/>
+      <c r="B142" s="81"/>
       <c r="C142" s="19">
         <v>3332210088</v>
       </c>
@@ -21497,7 +21527,7 @@
       <c r="A143" s="9">
         <v>141</v>
       </c>
-      <c r="B143" s="88"/>
+      <c r="B143" s="81"/>
       <c r="C143" s="19">
         <v>3332210091</v>
       </c>
@@ -21637,7 +21667,7 @@
       <c r="A144" s="9">
         <v>142</v>
       </c>
-      <c r="B144" s="88"/>
+      <c r="B144" s="81"/>
       <c r="C144" s="21">
         <v>3332210096</v>
       </c>
@@ -21776,7 +21806,7 @@
       <c r="A145" s="9">
         <v>143</v>
       </c>
-      <c r="B145" s="88"/>
+      <c r="B145" s="81"/>
       <c r="C145" s="21">
         <v>3332210056</v>
       </c>
@@ -21917,7 +21947,7 @@
       <c r="A146" s="9">
         <v>144</v>
       </c>
-      <c r="B146" s="88"/>
+      <c r="B146" s="81"/>
       <c r="C146" s="21">
         <v>3332210084</v>
       </c>
@@ -22058,7 +22088,7 @@
       <c r="A147" s="9">
         <v>145</v>
       </c>
-      <c r="B147" s="88"/>
+      <c r="B147" s="81"/>
       <c r="C147" s="19">
         <v>3332210043</v>
       </c>
@@ -22197,7 +22227,7 @@
       <c r="A148" s="9">
         <v>146</v>
       </c>
-      <c r="B148" s="88"/>
+      <c r="B148" s="81"/>
       <c r="C148" s="19">
         <v>3332210092</v>
       </c>
@@ -22336,7 +22366,7 @@
       <c r="A149" s="9">
         <v>147</v>
       </c>
-      <c r="B149" s="88"/>
+      <c r="B149" s="81"/>
       <c r="C149" s="19">
         <v>3332210099</v>
       </c>
@@ -22475,7 +22505,7 @@
       <c r="A150" s="9">
         <v>148</v>
       </c>
-      <c r="B150" s="88"/>
+      <c r="B150" s="81"/>
       <c r="C150" s="21">
         <v>3332210004</v>
       </c>
@@ -22500,23 +22530,23 @@
       </c>
       <c r="J150" s="30">
         <f t="shared" ref="J150:L150" ca="1" si="23">RANDBETWEEN(87,92)</f>
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K150" s="30">
         <f t="shared" ca="1" si="23"/>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="L150" s="30">
         <f t="shared" ca="1" si="23"/>
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="M150" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>62.5</v>
+        <v>63.1</v>
       </c>
       <c r="N150" s="30">
         <f t="shared" ref="N150:P150" ca="1" si="24">RANDBETWEEN(87,92)</f>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="O150" s="30">
         <f t="shared" ca="1" si="24"/>
@@ -22528,31 +22558,31 @@
       </c>
       <c r="Q150" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>62.2</v>
+        <v>62.8</v>
       </c>
       <c r="R150" s="30">
         <f t="shared" ref="R150:T150" ca="1" si="25">RANDBETWEEN(87,92)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="S150" s="30">
         <f t="shared" ca="1" si="25"/>
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="T150" s="30">
         <f t="shared" ca="1" si="25"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="U150" s="4">
         <f t="shared" ca="1" si="22"/>
-        <v>64.099999999999994</v>
+        <v>63.3</v>
       </c>
       <c r="V150" s="67">
         <f t="shared" ref="V150:X150" ca="1" si="26">RANDBETWEEN(87,92)</f>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W150" s="57">
         <f t="shared" ca="1" si="26"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="X150" s="57">
         <f t="shared" ca="1" si="26"/>
@@ -22560,66 +22590,66 @@
       </c>
       <c r="Y150" s="4">
         <f t="shared" ca="1" si="4"/>
-        <v>62.6</v>
+        <v>62.599999999999994</v>
       </c>
       <c r="Z150" s="67">
         <f t="shared" ref="Z150:AB150" ca="1" si="27">RANDBETWEEN(87,92)</f>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="AA150" s="57">
         <f t="shared" ca="1" si="27"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AB150" s="57">
         <f t="shared" ca="1" si="27"/>
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AC150" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>62.9</v>
+        <v>61.4</v>
       </c>
       <c r="AD150" s="67">
         <f t="shared" ref="AD150:AF150" ca="1" si="28">RANDBETWEEN(87,92)</f>
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AE150" s="57">
         <f t="shared" ca="1" si="28"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AF150" s="57">
         <f t="shared" ca="1" si="28"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG150" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>63.7</v>
+        <v>62.7</v>
       </c>
       <c r="AH150" s="67">
         <f t="shared" ref="AH150:AJ150" ca="1" si="29">RANDBETWEEN(87,92)</f>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AI150" s="57">
         <f t="shared" ca="1" si="29"/>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="AJ150" s="57">
         <f t="shared" ca="1" si="29"/>
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AK150" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>61.9</v>
+        <v>62.599999999999994</v>
       </c>
       <c r="AL150" s="9">
         <f t="shared" ca="1" si="16"/>
-        <v>62.912499999999994</v>
+        <v>62.737499999999997</v>
       </c>
       <c r="AM150" s="24">
         <v>84</v>
       </c>
       <c r="AN150" s="17">
         <f t="shared" ca="1" si="20"/>
-        <v>88.912499999999994</v>
+        <v>88.737499999999997</v>
       </c>
       <c r="AO150" s="4" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -22633,7 +22663,7 @@
       <c r="A151" s="9">
         <v>149</v>
       </c>
-      <c r="B151" s="88"/>
+      <c r="B151" s="81"/>
       <c r="C151" s="21">
         <v>3332210046</v>
       </c>
@@ -22658,39 +22688,39 @@
       </c>
       <c r="J151" s="30">
         <f t="shared" ref="J151:L151" ca="1" si="30">RANDBETWEEN(87,92)</f>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K151" s="30">
         <f t="shared" ca="1" si="30"/>
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L151" s="30">
         <f t="shared" ca="1" si="30"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M151" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>63.199999999999996</v>
+        <v>62.400000000000006</v>
       </c>
       <c r="N151" s="30">
         <f t="shared" ref="N151:P151" ca="1" si="31">RANDBETWEEN(87,92)</f>
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="O151" s="30">
         <f t="shared" ca="1" si="31"/>
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P151" s="30">
         <f t="shared" ca="1" si="31"/>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="Q151" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>62.4</v>
+        <v>62.8</v>
       </c>
       <c r="R151" s="30">
         <f t="shared" ref="R151:T151" ca="1" si="32">RANDBETWEEN(87,92)</f>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S151" s="30">
         <f t="shared" ca="1" si="32"/>
@@ -22698,19 +22728,19 @@
       </c>
       <c r="T151" s="30">
         <f t="shared" ca="1" si="32"/>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="U151" s="4">
         <f t="shared" ca="1" si="22"/>
-        <v>62.1</v>
+        <v>62.6</v>
       </c>
       <c r="V151" s="68">
         <f t="shared" ref="V151:X151" ca="1" si="33">RANDBETWEEN(87,92)</f>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W151" s="69">
         <f t="shared" ca="1" si="33"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="X151" s="69">
         <f t="shared" ca="1" si="33"/>
@@ -22722,7 +22752,7 @@
       </c>
       <c r="Z151" s="68">
         <f t="shared" ref="Z151:AB151" ca="1" si="34">RANDBETWEEN(87,92)</f>
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AA151" s="69">
         <f t="shared" ca="1" si="34"/>
@@ -22730,54 +22760,54 @@
       </c>
       <c r="AB151" s="69">
         <f t="shared" ca="1" si="34"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC151" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>62.900000000000006</v>
+        <v>63.4</v>
       </c>
       <c r="AD151" s="68">
         <f t="shared" ref="AD151:AF151" ca="1" si="35">RANDBETWEEN(87,92)</f>
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AE151" s="69">
         <f t="shared" ca="1" si="35"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AF151" s="69">
         <f t="shared" ca="1" si="35"/>
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="AG151" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>63</v>
+        <v>62.900000000000006</v>
       </c>
       <c r="AH151" s="68">
         <f t="shared" ref="AH151:AJ151" ca="1" si="36">RANDBETWEEN(87,92)</f>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AI151" s="69">
         <f t="shared" ca="1" si="36"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AJ151" s="69">
         <f t="shared" ca="1" si="36"/>
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AK151" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>63.300000000000004</v>
+        <v>63</v>
       </c>
       <c r="AL151" s="9">
         <f t="shared" ca="1" si="16"/>
-        <v>62.912500000000001</v>
+        <v>62.9375</v>
       </c>
       <c r="AM151" s="24">
         <v>83</v>
       </c>
       <c r="AN151" s="17">
         <f t="shared" ca="1" si="20"/>
-        <v>88.662499999999994</v>
+        <v>88.6875</v>
       </c>
       <c r="AO151" s="4" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -22795,7 +22825,7 @@
       <c r="A152" s="9">
         <v>150</v>
       </c>
-      <c r="B152" s="88"/>
+      <c r="B152" s="81"/>
       <c r="C152" s="21">
         <v>3332210054</v>
       </c>
@@ -22820,11 +22850,11 @@
       </c>
       <c r="J152" s="30">
         <f t="shared" ref="J152:L152" ca="1" si="37">RANDBETWEEN(87,92)</f>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K152" s="30">
         <f t="shared" ca="1" si="37"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L152" s="30">
         <f t="shared" ca="1" si="37"/>
@@ -22832,71 +22862,71 @@
       </c>
       <c r="M152" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>62.7</v>
+        <v>62.099999999999994</v>
       </c>
       <c r="N152" s="30">
         <f t="shared" ref="N152:P152" ca="1" si="38">RANDBETWEEN(87,92)</f>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O152" s="30">
         <f t="shared" ca="1" si="38"/>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="P152" s="30">
         <f t="shared" ca="1" si="38"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="Q152" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>62</v>
+        <v>62.800000000000004</v>
       </c>
       <c r="R152" s="30">
         <f t="shared" ref="R152:T152" ca="1" si="39">RANDBETWEEN(87,92)</f>
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="S152" s="30">
         <f t="shared" ca="1" si="39"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T152" s="30">
         <f t="shared" ca="1" si="39"/>
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="U152" s="4">
         <f t="shared" ca="1" si="22"/>
-        <v>63.800000000000004</v>
+        <v>62.5</v>
       </c>
       <c r="V152" s="68">
         <f t="shared" ref="V152:X152" ca="1" si="40">RANDBETWEEN(87,92)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W152" s="69">
         <f t="shared" ca="1" si="40"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X152" s="69">
         <f t="shared" ca="1" si="40"/>
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="Y152" s="4">
         <f t="shared" ca="1" si="4"/>
-        <v>62.6</v>
+        <v>63.4</v>
       </c>
       <c r="Z152" s="68">
         <f t="shared" ref="Z152:AB152" ca="1" si="41">RANDBETWEEN(87,92)</f>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA152" s="69">
         <f t="shared" ca="1" si="41"/>
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AB152" s="69">
         <f t="shared" ca="1" si="41"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AC152" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>61.899999999999991</v>
+        <v>62.6</v>
       </c>
       <c r="AD152" s="68">
         <f t="shared" ref="AD152:AF152" ca="1" si="42">RANDBETWEEN(87,92)</f>
@@ -22904,42 +22934,42 @@
       </c>
       <c r="AE152" s="69">
         <f t="shared" ca="1" si="42"/>
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AF152" s="69">
         <f t="shared" ca="1" si="42"/>
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AG152" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>62.900000000000006</v>
+        <v>61.899999999999991</v>
       </c>
       <c r="AH152" s="68">
         <f t="shared" ref="AH152:AJ152" ca="1" si="43">RANDBETWEEN(87,92)</f>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="AI152" s="69">
         <f t="shared" ca="1" si="43"/>
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="AJ152" s="69">
         <f t="shared" ca="1" si="43"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AK152" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>62.599999999999994</v>
+        <v>63.3</v>
       </c>
       <c r="AL152" s="9">
         <f t="shared" ca="1" si="16"/>
-        <v>62.662500000000009</v>
+        <v>62.674999999999997</v>
       </c>
       <c r="AM152" s="16">
         <v>84.5</v>
       </c>
       <c r="AN152" s="17">
         <f t="shared" ca="1" si="20"/>
-        <v>88.787500000000009</v>
+        <v>88.8</v>
       </c>
       <c r="AO152" s="4" t="str">
         <f t="shared" ca="1" si="9"/>
@@ -22953,7 +22983,7 @@
       <c r="A153" s="9">
         <v>151</v>
       </c>
-      <c r="B153" s="88"/>
+      <c r="B153" s="81"/>
       <c r="C153" s="19">
         <v>3332200052</v>
       </c>
@@ -23092,7 +23122,7 @@
       <c r="A154" s="9">
         <v>152</v>
       </c>
-      <c r="B154" s="88"/>
+      <c r="B154" s="81"/>
       <c r="C154" s="19">
         <v>3332200027</v>
       </c>
@@ -23227,7 +23257,7 @@
       <c r="A155" s="9">
         <v>153</v>
       </c>
-      <c r="B155" s="88"/>
+      <c r="B155" s="81"/>
       <c r="C155" s="19">
         <v>3332220073</v>
       </c>
@@ -23366,7 +23396,7 @@
       <c r="A156" s="9">
         <v>154</v>
       </c>
-      <c r="B156" s="88"/>
+      <c r="B156" s="81"/>
       <c r="C156" s="19">
         <v>3332200072</v>
       </c>
@@ -23505,7 +23535,7 @@
       <c r="A157" s="9">
         <v>155</v>
       </c>
-      <c r="B157" s="88"/>
+      <c r="B157" s="81"/>
       <c r="C157" s="21">
         <v>3332200091</v>
       </c>
@@ -23643,7 +23673,7 @@
       <c r="A158" s="9">
         <v>156</v>
       </c>
-      <c r="B158" s="88"/>
+      <c r="B158" s="81"/>
       <c r="C158" s="21">
         <v>3332200036</v>
       </c>
@@ -23780,7 +23810,7 @@
       <c r="A159" s="9">
         <v>157</v>
       </c>
-      <c r="B159" s="88"/>
+      <c r="B159" s="81"/>
       <c r="C159" s="21">
         <v>3332200037</v>
       </c>
@@ -23919,7 +23949,7 @@
       <c r="A160" s="9">
         <v>158</v>
       </c>
-      <c r="B160" s="88"/>
+      <c r="B160" s="81"/>
       <c r="C160" s="19">
         <v>3332200042</v>
       </c>
@@ -24058,7 +24088,7 @@
       <c r="A161" s="9">
         <v>159</v>
       </c>
-      <c r="B161" s="88"/>
+      <c r="B161" s="81"/>
       <c r="C161" s="19">
         <v>3332200115</v>
       </c>
@@ -24196,7 +24226,7 @@
       <c r="A162" s="9">
         <v>160</v>
       </c>
-      <c r="B162" s="88"/>
+      <c r="B162" s="81"/>
       <c r="C162" s="19">
         <v>3332200097</v>
       </c>
@@ -24335,7 +24365,7 @@
       <c r="A163" s="9">
         <v>161</v>
       </c>
-      <c r="B163" s="88"/>
+      <c r="B163" s="81"/>
       <c r="C163" s="21">
         <v>3332200005</v>
       </c>
@@ -24474,7 +24504,7 @@
       <c r="A164" s="9">
         <v>162</v>
       </c>
-      <c r="B164" s="88"/>
+      <c r="B164" s="81"/>
       <c r="C164" s="21">
         <v>3332200007</v>
       </c>
@@ -24613,7 +24643,7 @@
       <c r="A165" s="9">
         <v>163</v>
       </c>
-      <c r="B165" s="88"/>
+      <c r="B165" s="81"/>
       <c r="C165" s="21">
         <v>3332200009</v>
       </c>
@@ -24752,7 +24782,7 @@
       <c r="A166" s="9">
         <v>164</v>
       </c>
-      <c r="B166" s="88"/>
+      <c r="B166" s="81"/>
       <c r="C166" s="19">
         <v>3332200053</v>
       </c>
@@ -24894,7 +24924,7 @@
       <c r="A167" s="9">
         <v>165</v>
       </c>
-      <c r="B167" s="88"/>
+      <c r="B167" s="81"/>
       <c r="C167" s="19">
         <v>3332200079</v>
       </c>
@@ -25027,8 +25057,8 @@
       <c r="AP167" s="18">
         <v>5</v>
       </c>
-      <c r="AQ167" s="85"/>
-      <c r="AR167" s="84"/>
+      <c r="AQ167" s="87"/>
+      <c r="AR167" s="86"/>
       <c r="AS167" s="70"/>
       <c r="AT167" s="39"/>
     </row>
@@ -25036,7 +25066,7 @@
       <c r="A168" s="9">
         <v>166</v>
       </c>
-      <c r="B168" s="88"/>
+      <c r="B168" s="81"/>
       <c r="C168" s="19">
         <v>3332200099</v>
       </c>
@@ -25178,7 +25208,7 @@
       <c r="A169" s="9">
         <v>167</v>
       </c>
-      <c r="B169" s="88"/>
+      <c r="B169" s="81"/>
       <c r="C169" s="21">
         <v>3332200043</v>
       </c>
@@ -25190,7 +25220,7 @@
       </c>
       <c r="F169" s="30">
         <f t="shared" ref="F169:H169" ca="1" si="48">RANDBETWEEN(85,90)</f>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G169" s="30">
         <f t="shared" ca="1" si="48"/>
@@ -25198,15 +25228,15 @@
       </c>
       <c r="H169" s="30">
         <f t="shared" ca="1" si="48"/>
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I169" s="4">
         <f t="shared" ca="1" si="21"/>
-        <v>60.099999999999994</v>
+        <v>61</v>
       </c>
       <c r="J169" s="30">
         <f t="shared" ref="J169:L169" ca="1" si="49">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K169" s="30">
         <f t="shared" ca="1" si="49"/>
@@ -25214,35 +25244,35 @@
       </c>
       <c r="L169" s="30">
         <f t="shared" ca="1" si="49"/>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="M169" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>60</v>
+        <v>60.5</v>
       </c>
       <c r="N169" s="67">
         <f t="shared" ref="N169:P169" ca="1" si="50">RANDBETWEEN(85,90)</f>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="O169" s="57">
         <f t="shared" ca="1" si="50"/>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P169" s="57">
         <f t="shared" ca="1" si="50"/>
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="Q169" s="4">
         <f t="shared" ca="1" si="46"/>
-        <v>62.1</v>
+        <v>61.699999999999996</v>
       </c>
       <c r="R169" s="67">
         <f t="shared" ref="R169:T169" ca="1" si="51">RANDBETWEEN(85,90)</f>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="S169" s="57">
         <f t="shared" ca="1" si="51"/>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T169" s="57">
         <f t="shared" ca="1" si="51"/>
@@ -25250,11 +25280,11 @@
       </c>
       <c r="U169" s="4">
         <f t="shared" ca="1" si="22"/>
-        <v>60.7</v>
+        <v>60.4</v>
       </c>
       <c r="V169" s="67">
         <f t="shared" ref="V169:X169" ca="1" si="52">RANDBETWEEN(85,90)</f>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="W169" s="57">
         <f t="shared" ca="1" si="52"/>
@@ -25266,15 +25296,15 @@
       </c>
       <c r="Y169" s="4">
         <f t="shared" ca="1" si="47"/>
-        <v>59.9</v>
+        <v>60.800000000000004</v>
       </c>
       <c r="Z169" s="67">
         <f t="shared" ref="Z169:AB169" ca="1" si="53">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="AA169" s="57">
         <f t="shared" ca="1" si="53"/>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AB169" s="57">
         <f t="shared" ca="1" si="53"/>
@@ -25282,23 +25312,23 @@
       </c>
       <c r="AC169" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>60.499999999999993</v>
+        <v>62.3</v>
       </c>
       <c r="AD169" s="67">
         <f t="shared" ref="AD169:AF169" ca="1" si="54">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AE169" s="57">
         <f t="shared" ca="1" si="54"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AF169" s="57">
         <f t="shared" ca="1" si="54"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG169" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>59.9</v>
+        <v>60.7</v>
       </c>
       <c r="AH169" s="67">
         <f t="shared" ref="AH169:AJ169" ca="1" si="55">RANDBETWEEN(85,90)</f>
@@ -25306,26 +25336,26 @@
       </c>
       <c r="AI169" s="57">
         <f t="shared" ca="1" si="55"/>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AJ169" s="57">
         <f t="shared" ca="1" si="55"/>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AK169" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>61.8</v>
+        <v>60.2</v>
       </c>
       <c r="AL169" s="9">
         <f t="shared" ca="1" si="16"/>
-        <v>60.624999999999993</v>
+        <v>60.949999999999996</v>
       </c>
       <c r="AM169" s="24">
         <v>90</v>
       </c>
       <c r="AN169" s="17">
         <f t="shared" ca="1" si="20"/>
-        <v>88.125</v>
+        <v>88.449999999999989</v>
       </c>
       <c r="AO169" s="4" t="str">
         <f ca="1">IF(AN169&gt;=85.01, "A", IF(AN169&gt;=81, "A-", IF(AN169&gt;=76, "B+", IF(AN169&gt;=71, "B", IF(AN169&gt;=66, "B-", IF(AN169&gt;=61, "C+", IF(AN169&gt;=56, "C", IF(AN169&gt;=51, "D", IF(AN169&gt;=0, "E")))))))))</f>
@@ -25342,7 +25372,7 @@
       <c r="A170" s="9">
         <v>168</v>
       </c>
-      <c r="B170" s="88"/>
+      <c r="B170" s="81"/>
       <c r="C170" s="21">
         <v>3332200089</v>
       </c>
@@ -25354,7 +25384,7 @@
       </c>
       <c r="F170" s="30">
         <f t="shared" ref="F170:H170" ca="1" si="56">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G170" s="30">
         <f t="shared" ca="1" si="56"/>
@@ -25362,99 +25392,99 @@
       </c>
       <c r="H170" s="30">
         <f t="shared" ca="1" si="56"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I170" s="4">
         <f t="shared" ca="1" si="21"/>
-        <v>61.5</v>
+        <v>61.699999999999996</v>
       </c>
       <c r="J170" s="30">
         <f t="shared" ref="J170:L170" ca="1" si="57">RANDBETWEEN(85,90)</f>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K170" s="30">
         <f t="shared" ca="1" si="57"/>
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L170" s="30">
         <f t="shared" ca="1" si="57"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M170" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>60.8</v>
+        <v>60.5</v>
       </c>
       <c r="N170" s="68">
         <f t="shared" ref="N170:P170" ca="1" si="58">RANDBETWEEN(85,90)</f>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O170" s="69">
         <f t="shared" ca="1" si="58"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P170" s="69">
         <f t="shared" ca="1" si="58"/>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Q170" s="4">
         <f t="shared" ca="1" si="46"/>
-        <v>62.5</v>
+        <v>61.4</v>
       </c>
       <c r="R170" s="68">
         <f t="shared" ref="R170:T170" ca="1" si="59">RANDBETWEEN(85,90)</f>
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="S170" s="69">
         <f t="shared" ca="1" si="59"/>
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="T170" s="69">
         <f t="shared" ca="1" si="59"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="U170" s="4">
         <f t="shared" ca="1" si="22"/>
-        <v>60.8</v>
+        <v>61.699999999999996</v>
       </c>
       <c r="V170" s="68">
         <f t="shared" ref="V170:X170" ca="1" si="60">RANDBETWEEN(85,90)</f>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W170" s="69">
         <f t="shared" ca="1" si="60"/>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="X170" s="69">
         <f t="shared" ca="1" si="60"/>
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Y170" s="4">
         <f t="shared" ca="1" si="47"/>
-        <v>61.4</v>
+        <v>61.3</v>
       </c>
       <c r="Z170" s="68">
         <f t="shared" ref="Z170:AB170" ca="1" si="61">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AA170" s="69">
         <f t="shared" ca="1" si="61"/>
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="AB170" s="69">
         <f t="shared" ca="1" si="61"/>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AC170" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>60.5</v>
+        <v>61.2</v>
       </c>
       <c r="AD170" s="68">
         <f t="shared" ref="AD170:AF170" ca="1" si="62">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AE170" s="69">
         <f t="shared" ca="1" si="62"/>
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="AF170" s="69">
         <f t="shared" ca="1" si="62"/>
@@ -25462,34 +25492,34 @@
       </c>
       <c r="AG170" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>61.3</v>
+        <v>61.599999999999994</v>
       </c>
       <c r="AH170" s="68">
         <f t="shared" ref="AH170:AJ170" ca="1" si="63">RANDBETWEEN(85,90)</f>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AI170" s="69">
         <f t="shared" ca="1" si="63"/>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="AJ170" s="69">
         <f t="shared" ca="1" si="63"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AK170" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>61.4</v>
+        <v>60.6</v>
       </c>
       <c r="AL170" s="9">
         <f t="shared" ca="1" si="16"/>
-        <v>61.274999999999999</v>
+        <v>61.25</v>
       </c>
       <c r="AM170" s="24">
         <v>85</v>
       </c>
       <c r="AN170" s="17">
         <f t="shared" ca="1" si="20"/>
-        <v>87.525000000000006</v>
+        <v>87.5</v>
       </c>
       <c r="AO170" s="4" t="str">
         <f t="shared" ref="AO170:AO175" ca="1" si="64">IF(AN170&gt;=86, "A", IF(AN170&gt;=81, "A-", IF(AN170&gt;=76, "B+", IF(AN170&gt;=71, "B", IF(AN170&gt;=66, "B-", IF(AN170&gt;=61, "C+", IF(AN170&gt;=56, "C", IF(AN170&gt;=51, "D", IF(AN170&gt;=0, "E")))))))))</f>
@@ -25506,7 +25536,7 @@
       <c r="A171" s="9">
         <v>169</v>
       </c>
-      <c r="B171" s="88"/>
+      <c r="B171" s="81"/>
       <c r="C171" s="21">
         <v>3332200108</v>
       </c>
@@ -25522,55 +25552,55 @@
       </c>
       <c r="G171" s="30">
         <f t="shared" ca="1" si="65"/>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H171" s="30">
         <f t="shared" ca="1" si="65"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I171" s="4">
         <f t="shared" ca="1" si="21"/>
-        <v>61.999999999999993</v>
+        <v>62.300000000000004</v>
       </c>
       <c r="J171" s="30">
         <f t="shared" ref="J171:L171" ca="1" si="66">RANDBETWEEN(85,90)</f>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K171" s="30">
         <f t="shared" ca="1" si="66"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L171" s="30">
         <f t="shared" ca="1" si="66"/>
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M171" s="4">
         <f t="shared" ca="1" si="15"/>
-        <v>61.3</v>
+        <v>60.400000000000006</v>
       </c>
       <c r="N171" s="68">
         <f t="shared" ref="N171:P171" ca="1" si="67">RANDBETWEEN(85,90)</f>
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="O171" s="69">
         <f t="shared" ca="1" si="67"/>
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P171" s="69">
         <f t="shared" ca="1" si="67"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q171" s="4">
         <f t="shared" ca="1" si="46"/>
-        <v>61.699999999999996</v>
+        <v>61.5</v>
       </c>
       <c r="R171" s="68">
         <f t="shared" ref="R171:T171" ca="1" si="68">RANDBETWEEN(85,90)</f>
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="S171" s="69">
         <f t="shared" ca="1" si="68"/>
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T171" s="69">
         <f t="shared" ca="1" si="68"/>
@@ -25578,63 +25608,63 @@
       </c>
       <c r="U171" s="4">
         <f t="shared" ca="1" si="22"/>
-        <v>63</v>
+        <v>60.9</v>
       </c>
       <c r="V171" s="68">
         <f t="shared" ref="V171:X171" ca="1" si="69">RANDBETWEEN(85,90)</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="W171" s="69">
         <f t="shared" ca="1" si="69"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X171" s="69">
         <f t="shared" ca="1" si="69"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Y171" s="4">
         <f t="shared" ca="1" si="47"/>
-        <v>61.999999999999993</v>
+        <v>62.7</v>
       </c>
       <c r="Z171" s="68">
         <f t="shared" ref="Z171:AB171" ca="1" si="70">RANDBETWEEN(85,90)</f>
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AA171" s="69">
         <f t="shared" ca="1" si="70"/>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AB171" s="69">
         <f t="shared" ca="1" si="70"/>
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AC171" s="4">
         <f t="shared" ca="1" si="5"/>
-        <v>60.5</v>
+        <v>61.3</v>
       </c>
       <c r="AD171" s="68">
         <f t="shared" ref="AD171:AF171" ca="1" si="71">RANDBETWEEN(85,90)</f>
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AE171" s="69">
         <f t="shared" ca="1" si="71"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AF171" s="69">
         <f t="shared" ca="1" si="71"/>
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AG171" s="4">
         <f t="shared" ca="1" si="6"/>
-        <v>60.199999999999996</v>
+        <v>61.5</v>
       </c>
       <c r="AH171" s="68">
         <f t="shared" ref="AH171:AJ171" ca="1" si="72">RANDBETWEEN(85,90)</f>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AI171" s="69">
         <f t="shared" ca="1" si="72"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AJ171" s="69">
         <f t="shared" ca="1" si="72"/>
@@ -25642,18 +25672,18 @@
       </c>
       <c r="AK171" s="4">
         <f t="shared" ca="1" si="19"/>
-        <v>61.899999999999991</v>
+        <v>61.3</v>
       </c>
       <c r="AL171" s="9">
         <f t="shared" ca="1" si="16"/>
-        <v>61.574999999999989</v>
+        <v>61.487500000000004</v>
       </c>
       <c r="AM171" s="24">
         <v>86</v>
       </c>
       <c r="AN171" s="17">
         <f t="shared" ca="1" si="20"/>
-        <v>88.074999999999989</v>
+        <v>87.987500000000011</v>
       </c>
       <c r="AO171" s="4" t="str">
         <f t="shared" ca="1" si="64"/>
@@ -25670,7 +25700,7 @@
       <c r="A172" s="9">
         <v>170</v>
       </c>
-      <c r="B172" s="88"/>
+      <c r="B172" s="81"/>
       <c r="C172" s="19">
         <v>3332190072</v>
       </c>
@@ -25809,7 +25839,7 @@
       <c r="A173" s="9">
         <v>171</v>
       </c>
-      <c r="B173" s="88"/>
+      <c r="B173" s="81"/>
       <c r="C173" s="19">
         <v>3332190080</v>
       </c>
@@ -25951,7 +25981,7 @@
       <c r="A174" s="9">
         <v>172</v>
       </c>
-      <c r="B174" s="88"/>
+      <c r="B174" s="81"/>
       <c r="C174" s="19">
         <v>3332190082</v>
       </c>
@@ -26089,7 +26119,7 @@
       <c r="A175" s="9">
         <v>173</v>
       </c>
-      <c r="B175" s="88"/>
+      <c r="B175" s="81"/>
       <c r="C175" s="76">
         <v>3332170050</v>
       </c>

</xml_diff>